<commit_message>
advanced towards Figure 1
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index_emorragie_gravi.xlsx
+++ b/i_codebooks/00_index_emorragie_gravi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="194">
   <si>
     <t>status</t>
   </si>
@@ -55,9 +55,6 @@
     <t>g_intermediate</t>
   </si>
   <si>
-    <t>D3_events_DEATH</t>
-  </si>
-  <si>
     <t>ready</t>
   </si>
   <si>
@@ -451,9 +448,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>D3_study_cohort</t>
-  </si>
-  <si>
     <t>D4_Cube_persontime_bleeding D3_source_population</t>
   </si>
   <si>
@@ -493,12 +487,6 @@
     <t>D5_Figure_IR</t>
   </si>
   <si>
-    <t>uninterrupted periods of treatment with the medicines of interest</t>
-  </si>
-  <si>
-    <t>episodes of bleeding occurring in the persons treated with the medicines of interest</t>
-  </si>
-  <si>
     <t>dynamic cohort of treated and at risk of bleeding</t>
   </si>
   <si>
@@ -511,15 +499,9 @@
     <t>D3_PERSONS D3_output_spells_category D3_dispensings_DOACs</t>
   </si>
   <si>
-    <t>D3_PERSONS D3_output_spells_category D3_persons_with_MoI</t>
-  </si>
-  <si>
     <t>persons with at least a dispensing of a Medicine of Interest during the study period</t>
   </si>
   <si>
-    <t>D3_dispensings_DOACs PRODUCTS D3_clean_spells</t>
-  </si>
-  <si>
     <t>conceptsetdataset D3_persons_with_MoI</t>
   </si>
   <si>
@@ -532,9 +514,6 @@
     <t>dynamic cohort of persons with bleeding</t>
   </si>
   <si>
-    <t>01_T2_60_selection_criteria_from_PERSON_to_persons_with_MoI</t>
-  </si>
-  <si>
     <t>D3_selection_criteria_from_persons_with_MoI_to_study_population</t>
   </si>
   <si>
@@ -559,48 +538,6 @@
     <t>D4_persons_with_MoI</t>
   </si>
   <si>
-    <t>03_T2_10_create_episodes_of_treatement</t>
-  </si>
-  <si>
-    <t>03_T2_20_create_bleeding_events</t>
-  </si>
-  <si>
-    <t>04_T3_10_create_source_population</t>
-  </si>
-  <si>
-    <t>05_T2_10_selection_criteria_from_persons_with_MoI_to_study_population</t>
-  </si>
-  <si>
-    <t>06_T3_10_create_study_population</t>
-  </si>
-  <si>
-    <t>07_T2_10_create_comorbodity</t>
-  </si>
-  <si>
-    <t>07_T2_20_create_comedication</t>
-  </si>
-  <si>
-    <t>07_T2_30_create_covariates_for_source_population</t>
-  </si>
-  <si>
-    <t>07_T2_40_create_covariates_for_study_population</t>
-  </si>
-  <si>
-    <t>08_T3_10_create_persontime_bleeding</t>
-  </si>
-  <si>
-    <t>08_T3_20_apply_Cube_to_persontime_bleeding</t>
-  </si>
-  <si>
-    <t>08_T3_30_create_persontime_bleeding_period</t>
-  </si>
-  <si>
-    <t>08_T3_40_apply_Cube_to_persontime_bleeding</t>
-  </si>
-  <si>
-    <t>09_T4_30_create_D5_IR</t>
-  </si>
-  <si>
     <t>09_T5_35_create_Figure_1</t>
   </si>
   <si>
@@ -608,6 +545,63 @@
   </si>
   <si>
     <t>incidence rate of bleeding in the source population, per trimester, gender, and ageband</t>
+  </si>
+  <si>
+    <t>01_T2_60_create_episodes_of_treatement</t>
+  </si>
+  <si>
+    <t>episodes of bleeding occurring in the persons treated with the MoI</t>
+  </si>
+  <si>
+    <t>01_T2_70_create_bleeding_events</t>
+  </si>
+  <si>
+    <t>01_T2_80_selection_criteria_from_PERSON_to_persons_with_MoI</t>
+  </si>
+  <si>
+    <t>D4_study_cohort</t>
+  </si>
+  <si>
+    <t>03_T3_10_create_source_population</t>
+  </si>
+  <si>
+    <t>04_T2_10_selection_criteria_from_persons_with_MoI_to_study_population</t>
+  </si>
+  <si>
+    <t>05_T3_10_create_study_population</t>
+  </si>
+  <si>
+    <t>06_T2_10_create_comorbodity</t>
+  </si>
+  <si>
+    <t>06_T2_20_create_comedication</t>
+  </si>
+  <si>
+    <t>06_T2_30_create_covariates_for_source_population</t>
+  </si>
+  <si>
+    <t>06_T2_40_create_covariates_for_study_population</t>
+  </si>
+  <si>
+    <t>07_T3_10_create_persontime_bleeding</t>
+  </si>
+  <si>
+    <t>07_T3_20_apply_Cube_to_persontime_bleeding</t>
+  </si>
+  <si>
+    <t>07_T3_30_create_persontime_bleeding_period</t>
+  </si>
+  <si>
+    <t>07_T3_40_apply_Cube_to_persontime_bleeding</t>
+  </si>
+  <si>
+    <t>08_T4_30_create_D5_IR</t>
+  </si>
+  <si>
+    <t>uninterrupted periods of treatment with the medicines of interest (MoI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3_dispensings_DOACs PRODUCTS </t>
   </si>
 </sst>
 </file>
@@ -1072,13 +1066,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>2</v>
@@ -1123,32 +1117,32 @@
         <v>7</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="13" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>10</v>
@@ -1165,7 +1159,7 @@
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="13" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>10</v>
@@ -1173,146 +1167,146 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="G6" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="G8" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="20"/>
       <c r="E9" s="14" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>179</v>
+        <v>171</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>170</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F11" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>159</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="C12" s="18"/>
       <c r="D12" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="C13" s="18"/>
+        <v>179</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>163</v>
+      </c>
       <c r="D13" s="13" t="s">
         <v>182</v>
       </c>
       <c r="F13" s="16"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="D14" s="13" t="s">
+      <c r="B14" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>184</v>
@@ -1320,10 +1314,10 @@
     </row>
     <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>185</v>
@@ -1331,58 +1325,59 @@
     </row>
     <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>153</v>
+        <v>162</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>165</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="D18" s="22" t="s">
+      <c r="B18" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F18" s="14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>145</v>
-      </c>
       <c r="D19" s="17" t="s">
         <v>188</v>
       </c>
       <c r="F19" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="23" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D20" s="17" t="s">
+      <c r="C20" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="22" t="s">
         <v>189</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>145</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="C21" s="22"/>
       <c r="D21" s="22" t="s">
         <v>190</v>
       </c>
@@ -1390,51 +1385,39 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22" t="s">
+    <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="F22" s="14" t="s">
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="16" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B24" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>193</v>
+      <c r="D25" s="17" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B25:C1048576 B1:C4 C21:C24 B10:C18 B7:C7 C9 B5:B6 B8:B9">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="B24:C1048576 B1:C4 C20:C23 B11:C17 B7:C9 B5:B6 B10">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1461,1139 +1444,1139 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
         <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
         <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
         <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
         <v>51</v>
       </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="B27" t="s">
-        <v>60</v>
-      </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B66" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B72" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B78" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B80" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B82" t="s">
         <v>116</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>117</v>
-      </c>
-      <c r="C82" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B85" t="s">
+        <v>122</v>
+      </c>
+      <c r="C85" t="s">
         <v>121</v>
       </c>
-      <c r="B85" t="s">
-        <v>123</v>
-      </c>
-      <c r="C85" t="s">
-        <v>122</v>
-      </c>
       <c r="D85" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B86" t="s">
+        <v>123</v>
+      </c>
+      <c r="C86" t="s">
         <v>121</v>
       </c>
-      <c r="B86" t="s">
-        <v>124</v>
-      </c>
-      <c r="C86" t="s">
-        <v>122</v>
-      </c>
       <c r="D86" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B87" t="s">
+        <v>124</v>
+      </c>
+      <c r="C87" t="s">
         <v>121</v>
       </c>
-      <c r="B87" t="s">
-        <v>125</v>
-      </c>
-      <c r="C87" t="s">
-        <v>122</v>
-      </c>
       <c r="D87" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B88" t="s">
+        <v>125</v>
+      </c>
+      <c r="C88" t="s">
         <v>121</v>
       </c>
-      <c r="B88" t="s">
-        <v>126</v>
-      </c>
-      <c r="C88" t="s">
-        <v>122</v>
-      </c>
       <c r="D88" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B89" t="s">
+        <v>126</v>
+      </c>
+      <c r="C89" t="s">
         <v>121</v>
       </c>
-      <c r="B89" t="s">
-        <v>127</v>
-      </c>
-      <c r="C89" t="s">
-        <v>122</v>
-      </c>
       <c r="D89" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B90" t="s">
+        <v>127</v>
+      </c>
+      <c r="C90" t="s">
         <v>121</v>
       </c>
-      <c r="B90" t="s">
-        <v>128</v>
-      </c>
-      <c r="C90" t="s">
-        <v>122</v>
-      </c>
       <c r="D90" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B91" t="s">
+        <v>128</v>
+      </c>
+      <c r="C91" t="s">
         <v>121</v>
       </c>
-      <c r="B91" t="s">
-        <v>129</v>
-      </c>
-      <c r="C91" t="s">
-        <v>122</v>
-      </c>
       <c r="D91" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B92" t="s">
+        <v>129</v>
+      </c>
+      <c r="C92" t="s">
         <v>121</v>
       </c>
-      <c r="B92" t="s">
-        <v>130</v>
-      </c>
-      <c r="C92" t="s">
-        <v>122</v>
-      </c>
       <c r="D92" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B93" t="s">
+        <v>130</v>
+      </c>
+      <c r="C93" t="s">
         <v>121</v>
       </c>
-      <c r="B93" t="s">
-        <v>131</v>
-      </c>
-      <c r="C93" t="s">
-        <v>122</v>
-      </c>
       <c r="D93" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B94" t="s">
+        <v>131</v>
+      </c>
+      <c r="C94" t="s">
         <v>121</v>
       </c>
-      <c r="B94" t="s">
-        <v>132</v>
-      </c>
-      <c r="C94" t="s">
-        <v>122</v>
-      </c>
       <c r="D94" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B95" t="s">
+        <v>132</v>
+      </c>
+      <c r="C95" t="s">
         <v>121</v>
       </c>
-      <c r="B95" t="s">
-        <v>133</v>
-      </c>
-      <c r="C95" t="s">
-        <v>122</v>
-      </c>
       <c r="D95" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B96" t="s">
+        <v>133</v>
+      </c>
+      <c r="C96" t="s">
         <v>121</v>
       </c>
-      <c r="B96" t="s">
+      <c r="D96" t="s">
         <v>134</v>
-      </c>
-      <c r="C96" t="s">
-        <v>122</v>
-      </c>
-      <c r="D96" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="97" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D97" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2603,12 +2586,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2863,21 +2849,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2902,18 +2894,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
first version for test
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index_emorragie_gravi.xlsx
+++ b/i_codebooks/00_index_emorragie_gravi.xlsx
@@ -493,9 +493,6 @@
     <t>D3_dispensings_DOACs</t>
   </si>
   <si>
-    <t>D3_episodes_of_treatment D3_bleeding_events D3_dispensings_DOACs D3_clean_spells</t>
-  </si>
-  <si>
     <t>D3_PERSONS D3_output_spells_category D3_dispensings_DOACs</t>
   </si>
   <si>
@@ -602,6 +599,9 @@
   </si>
   <si>
     <t xml:space="preserve">D3_dispensings_DOACs PRODUCTS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3_episodes_of_treatment D3_bleeding_events </t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -677,6 +677,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -690,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -731,6 +737,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1069,10 +1081,10 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1126,7 +1138,7 @@
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>16</v>
@@ -1159,7 +1171,7 @@
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>10</v>
@@ -1173,7 +1185,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1184,7 +1196,7 @@
         <v>156</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>15</v>
@@ -1198,13 +1210,13 @@
         <v>138</v>
       </c>
       <c r="C7" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" s="14" t="s">
         <v>192</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>193</v>
       </c>
       <c r="G7" s="15"/>
     </row>
@@ -1213,13 +1225,13 @@
         <v>149</v>
       </c>
       <c r="C8" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>177</v>
-      </c>
       <c r="F8" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>15</v>
@@ -1227,11 +1239,11 @@
     </row>
     <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>10</v>
@@ -1242,16 +1254,16 @@
     </row>
     <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1262,31 +1274,31 @@
         <v>155</v>
       </c>
       <c r="D11" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="F11" s="16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="13" t="s">
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>181</v>
-      </c>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>182</v>
       </c>
       <c r="F13" s="16"/>
     </row>
@@ -1298,7 +1310,7 @@
         <v>147</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1309,7 +1321,7 @@
         <v>148</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1320,18 +1332,18 @@
         <v>151</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1342,7 +1354,7 @@
         <v>143</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>150</v>
@@ -1353,7 +1365,7 @@
         <v>137</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>136</v>
@@ -1367,7 +1379,7 @@
         <v>143</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>150</v>
@@ -1379,7 +1391,7 @@
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>152</v>
@@ -1387,13 +1399,13 @@
     </row>
     <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>174</v>
-      </c>
       <c r="D23" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
@@ -1409,7 +1421,7 @@
         <v>154</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2586,15 +2598,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2849,27 +2858,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2894,9 +2897,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
complete to test Figure 1
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index_emorragie_gravi.xlsx
+++ b/i_codebooks/00_index_emorragie_gravi.xlsx
@@ -1081,10 +1081,10 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2598,12 +2598,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2858,21 +2861,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2897,18 +2906,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update codebooks for statistical analysis
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index_emorragie_gravi.xlsx
+++ b/i_codebooks/00_index_emorragie_gravi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="201">
   <si>
     <t>status</t>
   </si>
@@ -602,6 +602,27 @@
   </si>
   <si>
     <t xml:space="preserve">D3_episodes_of_treatment D3_bleeding_events </t>
+  </si>
+  <si>
+    <t>D4_analytic_dataset</t>
+  </si>
+  <si>
+    <t>episode of bleeding including outcomes and covariates</t>
+  </si>
+  <si>
+    <t>07_T3_50_create_analytic_dataset</t>
+  </si>
+  <si>
+    <t>D5_results_from_analysis</t>
+  </si>
+  <si>
+    <t>08_T4_40_analysis</t>
+  </si>
+  <si>
+    <t>01_T2_90_create_dispensings_AA</t>
+  </si>
+  <si>
+    <t>D3_dispensings_AA</t>
   </si>
 </sst>
 </file>
@@ -644,9 +665,10 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -683,6 +705,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -696,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -743,6 +771,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1078,13 +1113,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1252,183 +1287,224 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C11" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D11" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F11" s="14" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="18" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C12" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D12" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F12" s="16" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25" t="s">
+      <c r="C13" s="24"/>
+      <c r="D13" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="24" t="s">
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C14" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D14" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C15" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D15" s="22" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C18" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D18" s="22" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
+    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C19" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D19" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F19" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D20" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F20" s="14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="23" t="s">
+    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C21" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D21" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F21" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="23" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22" t="s">
+      <c r="C22" s="22"/>
+      <c r="D22" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F22" s="14" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="16"/>
+    </row>
+    <row r="26" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B26" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C26" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D26" s="17" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="16"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F29" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="16" t="s">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D30" s="17" t="s">
         <v>171</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C18">
+  <conditionalFormatting sqref="C19">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:C1048576 B1:C4 C20:C23 B11:C17 B7:C9 B5:B6 B10">
+  <conditionalFormatting sqref="B29:C1048576 B1:C4 C21:C23 B12:C18 B7:C10 B5:B6 B11 C25:C28">
     <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2610,6 +2686,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2860,15 +2945,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
@@ -2887,6 +2963,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2903,12 +2987,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated simulated analytical dataset
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index_emorragie_gravi.xlsx
+++ b/i_codebooks/00_index_emorragie_gravi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="211">
   <si>
     <t>status</t>
   </si>
@@ -682,6 +682,15 @@
       </rPr>
       <t>D4_persons_with_MoI</t>
     </r>
+  </si>
+  <si>
+    <t>D3_outcomes</t>
+  </si>
+  <si>
+    <t>study outcomes</t>
+  </si>
+  <si>
+    <t>06_T2_50_create_study_outcomes</t>
   </si>
 </sst>
 </file>
@@ -1197,13 +1206,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1497,128 +1506,139 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C21" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D21" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F21" s="14" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="14" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D22" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F22" s="14" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="23" t="s">
+    <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C23" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D23" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F23" s="14" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="23" t="s">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22" t="s">
+      <c r="C24" s="22"/>
+      <c r="D24" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F24" s="14" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
+    <row r="25" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C25" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D25" s="17" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="14" t="s">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D26" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F26" s="12" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B26" s="16" t="s">
+    <row r="27" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C27" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D27" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F27" s="14" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="16" t="s">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D28" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F28" s="14" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="14" t="s">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F29" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="16" t="s">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D30" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F30" s="14" t="s">
         <v>166</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C20">
+  <conditionalFormatting sqref="C21">
     <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28:C1048576 B6:C7 B5 B8 C22:C27 B1:C4 B9:C19">
+  <conditionalFormatting sqref="B29:C1048576 B6:C7 B5 B8 C23:C28 B1:C4 B9:C20">
     <cfRule type="duplicateValues" dxfId="3" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
@@ -2797,27 +2817,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -3068,32 +3067,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3110,4 +3105,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
setting the stage to compute covariates
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index_emorragie_gravi.xlsx
+++ b/i_codebooks/00_index_emorragie_gravi.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="104">
   <si>
     <t>status</t>
   </si>
@@ -112,9 +112,6 @@
     <t>D3_source_population_with_covariates</t>
   </si>
   <si>
-    <t>comorbidity in the source population, as TD dataset</t>
-  </si>
-  <si>
     <t>comedications in the source population, as TD dataset</t>
   </si>
   <si>
@@ -194,15 +191,6 @@
   </si>
   <si>
     <t>03_T3_10_create_source_population</t>
-  </si>
-  <si>
-    <t>06_T2_20_create_comedication</t>
-  </si>
-  <si>
-    <t>06_T2_30_create_covariates_for_source_population</t>
-  </si>
-  <si>
-    <t>06_T2_40_create_covariates_for_study_population</t>
   </si>
   <si>
     <t>07_T3_10_create_persontime_bleeding</t>
@@ -348,13 +336,78 @@
     <t>06_T2_50_create_study_outcomes</t>
   </si>
   <si>
-    <t>06_T2_10_create_comorbidity</t>
-  </si>
-  <si>
-    <t>D3_TD_condition</t>
-  </si>
-  <si>
-    <t>D3_TD_variable_comedication</t>
+    <t>03_conceptset.R</t>
+  </si>
+  <si>
+    <r>
+      <t>D3_TD_</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF444444"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>condition</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D3_TD_variable_</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF444444"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>comedication</t>
+    </r>
+  </si>
+  <si>
+    <t>TD_variables_condition</t>
+  </si>
+  <si>
+    <t>5_variable_list</t>
+  </si>
+  <si>
+    <t>TD_variables_medication</t>
+  </si>
+  <si>
+    <t>06_T2_60_create_comorbidity</t>
+  </si>
+  <si>
+    <t>06_T2_70_create_comedication</t>
+  </si>
+  <si>
+    <t>06_T2_80_create_covariates_for_source_population</t>
+  </si>
+  <si>
+    <t>06_T2_90_create_covariates_for_study_population</t>
+  </si>
+  <si>
+    <t>comorbidity in the source population as TD dataset</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">D3_source_population 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conceptsetdataset</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -500,7 +553,17 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -864,10 +927,10 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -921,13 +984,13 @@
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>12</v>
@@ -939,13 +1002,13 @@
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G3" s="12"/>
     </row>
@@ -958,13 +1021,13 @@
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -972,10 +1035,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>12</v>
@@ -989,23 +1052,23 @@
         <v>23</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>10</v>
@@ -1016,16 +1079,16 @@
     </row>
     <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1033,13 +1096,13 @@
         <v>25</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>12</v>
@@ -1047,96 +1110,102 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="10"/>
       <c r="F11" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B16" s="22" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="22" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>58</v>
+        <v>99</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="29" x14ac:dyDescent="0.35">
@@ -1144,32 +1213,32 @@
         <v>29</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="29" x14ac:dyDescent="0.35">
@@ -1180,10 +1249,10 @@
         <v>28</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
@@ -1191,7 +1260,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>21</v>
@@ -1199,61 +1268,61 @@
     </row>
     <row r="23" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B27" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>53</v>
-      </c>
       <c r="D27" s="14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>22</v>
@@ -1261,13 +1330,13 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
@@ -1280,30 +1349,30 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C21">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C1048576 B6:C7 B5 B8 C23:C28 B1:C4 B9:C20">
-    <cfRule type="duplicateValues" dxfId="3" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
+  <conditionalFormatting sqref="F13">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1315,10 +1384,10 @@
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1343,107 +1412,208 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="C2" s="3"/>
+      <c r="D2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
+      <c r="D16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
+      <c r="D19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
+      <c r="D21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
@@ -1635,6 +1805,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -1885,42 +2076,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1943,9 +2102,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>